<commit_message>
Refresh name to match Zimbabwe
</commit_message>
<xml_diff>
--- a/AppSource Deneb maps/Countries.xlsx
+++ b/AppSource Deneb maps/Countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\data-visualisation-datasets\AppSource Deneb maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3227CDF3-69EE-4C0C-88CE-E5B06EA17F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CCF7C3-9520-4990-84FB-FA5404FE5F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="2970" windowWidth="18255" windowHeight="10470" xr2:uid="{9CF71F7C-3F44-4075-BFD8-9A836617284E}"/>
+    <workbookView xWindow="720" yWindow="4740" windowWidth="18255" windowHeight="10470" xr2:uid="{9CF71F7C-3F44-4075-BFD8-9A836617284E}"/>
   </bookViews>
   <sheets>
     <sheet name="Country" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -926,7 +925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FD3A53-00A0-40F4-A82A-6D0ED86980EC}">
   <dimension ref="A1:A175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Merge names from map source
</commit_message>
<xml_diff>
--- a/AppSource Deneb maps/Countries.xlsx
+++ b/AppSource Deneb maps/Countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\data-visualisation-datasets\AppSource Deneb maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CCF7C3-9520-4990-84FB-FA5404FE5F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A353F65-0B9F-427B-A813-459B883872C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="4740" windowWidth="18255" windowHeight="10470" xr2:uid="{9CF71F7C-3F44-4075-BFD8-9A836617284E}"/>
+    <workbookView xWindow="-15" yWindow="7650" windowWidth="7170" windowHeight="11145" xr2:uid="{9CF71F7C-3F44-4075-BFD8-9A836617284E}"/>
   </bookViews>
   <sheets>
     <sheet name="Country" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:A175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>